<commit_message>
Fix bonus not showing. Fix scoring for wave entry enemies. Fix convoy scoring.
</commit_message>
<xml_diff>
--- a/memory_map.xlsx
+++ b/memory_map.xlsx
@@ -15,7 +15,7 @@
   </definedNames>
   <calcPr calcId="124519"/>
   <pivotCaches>
-    <pivotCache cacheId="10" r:id="rId3"/>
+    <pivotCache cacheId="15" r:id="rId3"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -620,7 +620,18 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="12">
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
     <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
     </dxf>
@@ -660,7 +671,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Nick" refreshedDate="44457.692029745369" createdVersion="3" refreshedVersion="3" minRefreshableVersion="3" recordCount="176">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Nick" refreshedDate="44457.692804513892" createdVersion="3" refreshedVersion="3" minRefreshableVersion="3" recordCount="176">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:I1048576" sheet="Data"/>
   </cacheSource>
@@ -3011,7 +3022,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
   <location ref="A3:C109" firstHeaderRow="2" firstDataRow="2" firstDataCol="2" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="9">
     <pivotField compact="0" outline="0" showAll="0"/>
@@ -3839,13 +3850,13 @@
     <dataField name="Sum of Used" fld="6" baseField="0" baseItem="0" numFmtId="3"/>
   </dataFields>
   <formats count="3">
-    <format dxfId="8">
+    <format dxfId="11">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="7">
+    <format dxfId="10">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="6">
+    <format dxfId="9">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
@@ -4144,8 +4155,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S393"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K47" sqref="K47"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A65" sqref="A65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4387,7 +4398,7 @@
         <v>1</v>
       </c>
       <c r="I5">
-        <f t="shared" si="9"/>
+        <f>I4+1</f>
         <v>4</v>
       </c>
       <c r="K5">
@@ -17254,8 +17265,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AM124"/>
   <sheetViews>
-    <sheetView topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="B128" sqref="B128"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="C69" sqref="C68:C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>